<commit_message>
Fix optimalisatie 2e variant; update meetresultaten
</commit_message>
<xml_diff>
--- a/Meetresultaten.xlsx
+++ b/Meetresultaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Uitvoeringstijd" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>punten=</t>
   </si>
@@ -114,12 +114,18 @@
   <si>
     <t>uitvoeringstijd:</t>
   </si>
+  <si>
+    <t>2e na optimalisatie:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2e na optimalisatie: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +149,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,6 +207,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,6 +868,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1182,6 +1198,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1299,6 +1316,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2829,7 +2847,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3012,7 +3029,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3130,7 +3146,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3291,7 +3306,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3509,7 +3523,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3627,7 +3640,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3783,7 +3795,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3990,7 +4001,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4108,7 +4118,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4730,7 +4739,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4936,7 +4944,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5054,7 +5061,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10180,13 +10186,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10218,7 +10224,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10741,10 +10747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10864,6 +10870,35 @@
         <v>1477</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="12">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12">
+        <v>13</v>
+      </c>
+      <c r="F5" s="12">
+        <v>19</v>
+      </c>
+      <c r="G5" s="12">
+        <v>35</v>
+      </c>
+      <c r="H5" s="12">
+        <v>99</v>
+      </c>
+      <c r="I5" s="12">
+        <v>131</v>
+      </c>
+    </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
@@ -11004,93 +11039,151 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
-        <v>1000</v>
-      </c>
-      <c r="E14">
-        <v>10000</v>
-      </c>
-      <c r="F14">
-        <v>100000</v>
-      </c>
-      <c r="G14">
-        <v>1000000</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="12">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12">
+        <v>3</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12">
+        <v>2</v>
+      </c>
+      <c r="F13" s="12">
+        <v>2</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2</v>
+      </c>
+      <c r="I13" s="12">
+        <v>2</v>
+      </c>
+      <c r="J13" s="12">
+        <v>2</v>
+      </c>
+      <c r="K13" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D15">
-        <v>26</v>
+        <v>1000</v>
       </c>
       <c r="E15">
-        <v>482</v>
+        <v>10000</v>
       </c>
       <c r="F15">
-        <v>48212</v>
+        <v>100000</v>
+      </c>
+      <c r="G15">
+        <v>1000000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>482</v>
       </c>
       <c r="F16">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>58</v>
+        <v>48212</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>7</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>12</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>144</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>2203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>42</v>
+      </c>
+      <c r="G19">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -17244,7 +17337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>

</xml_diff>